<commit_message>
đang làm hiển thị cmt
</commit_message>
<xml_diff>
--- a/EC_proposal_C2C.xlsx
+++ b/EC_proposal_C2C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eCommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2F227C-A933-4A89-80F1-6FC9DB7B7510}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA98C41-B50B-4DD5-AF44-9362F961AD89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{15EB6947-BFCB-2C40-A24F-74282B3BE957}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>....</t>
   </si>
@@ -269,9 +269,6 @@
   <si>
     <t xml:space="preserve"> - Được cập nhập thủ công khi phát sinh lỗi 
  - Có chức năng thu phí: Sau khi nhận tiền, tiến hành active chức năng đăng bài của tài khoản, cùng với thời gian mà người bán đăng kí. Trước khi hết hạn, gửi thông báo qua tài khoản người bán, chặn chức năng bài khi tài khoản hết hạn.</t>
-  </si>
-  <si>
-    <t>ko được lưu số tài khoản của người khác</t>
   </si>
 </sst>
 </file>
@@ -473,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -534,21 +531,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -570,17 +579,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B921C1C-7DF0-C64F-B9A4-BF857010D7F8}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -914,15 +914,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
@@ -939,10 +939,10 @@
         <v>27</v>
       </c>
       <c r="D3" s="15"/>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="31"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -954,8 +954,8 @@
         <v>36</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
       <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -967,8 +967,8 @@
         <v>37</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -980,8 +980,8 @@
         <v>38</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -989,8 +989,8 @@
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -998,11 +998,11 @@
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="2"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
@@ -1010,10 +1010,10 @@
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="8"/>
       <c r="E10" s="10" t="s">
         <v>39</v>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
         <v>40</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="2"/>
       <c r="E12" s="4" t="s">
         <v>41</v>
@@ -1049,10 +1049,10 @@
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="2"/>
       <c r="E13" s="4" t="s">
         <v>42</v>
@@ -1061,11 +1061,11 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="s">
         <v>48</v>
@@ -1074,33 +1074,33 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="204" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="2"/>
       <c r="E17" s="19" t="s">
         <v>50</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="2"/>
       <c r="E18" s="4" t="s">
         <v>51</v>
@@ -1125,10 +1125,10 @@
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="2"/>
       <c r="E19" s="4" t="s">
         <v>52</v>
@@ -1138,10 +1138,10 @@
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="2"/>
       <c r="E20" s="4" t="s">
         <v>44</v>
@@ -1151,10 +1151,10 @@
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="2"/>
       <c r="E21" s="4"/>
       <c r="F21" s="3"/>
@@ -1188,10 +1188,10 @@
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="2"/>
       <c r="E24" s="4" t="s">
         <v>55</v>
@@ -1201,10 +1201,10 @@
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="2"/>
       <c r="E25" s="4" t="s">
         <v>57</v>
@@ -1214,10 +1214,10 @@
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="37"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="2"/>
       <c r="E26" s="4" t="s">
         <v>58</v>
@@ -1233,22 +1233,22 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="37"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="2"/>
       <c r="E29" s="19" t="s">
         <v>59</v>
@@ -1271,10 +1271,10 @@
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="26"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="2"/>
       <c r="E31" s="4" t="s">
         <v>60</v>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="26"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="2"/>
       <c r="E32" s="4" t="s">
         <v>46</v>
@@ -1309,22 +1309,22 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="1:7" s="1" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="37"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="2"/>
       <c r="E35" s="19" t="s">
         <v>65</v>
@@ -1334,10 +1334,10 @@
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="37"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="2"/>
       <c r="E36" s="19" t="s">
         <v>63</v>
@@ -1349,10 +1349,10 @@
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="37"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="2"/>
       <c r="E37" s="19" t="s">
         <v>56</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="37"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="2"/>
       <c r="E38" s="19" t="s">
         <v>64</v>
@@ -1384,22 +1384,22 @@
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" spans="1:7" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="37"/>
+      <c r="C41" s="23"/>
       <c r="D41" s="2"/>
       <c r="E41" s="4" t="s">
         <v>47</v>
@@ -1409,10 +1409,10 @@
     </row>
     <row r="42" spans="1:7" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="37"/>
+      <c r="C42" s="23"/>
       <c r="D42" s="2"/>
       <c r="E42" s="4" t="s">
         <v>43</v>
@@ -1422,35 +1422,31 @@
     </row>
     <row r="43" spans="1:7" s="1" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="26"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="2"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
       <c r="G43" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="26"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="A28:G28"/>
@@ -1465,16 +1461,18 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="0.58000000000000007" bottom="0.59055118110236227" header="0.37" footer="0.6100000000000001"/>
   <pageSetup paperSize="9" scale="99" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>